<commit_message>
data: add 2023-05-12 notices
</commit_message>
<xml_diff>
--- a/data/st_notices/2023-05-10_ST股公告(截至22:42:24).xlsx
+++ b/data/st_notices/2023-05-10_ST股公告(截至22:42:24).xlsx
@@ -1237,10 +1237,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1273,15 +1273,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1303,31 +1319,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1341,6 +1342,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1356,23 +1358,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1387,14 +1380,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1408,9 +1409,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1425,7 +1425,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1437,7 +1455,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,31 +1527,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1485,127 +1605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1634,6 +1634,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1658,30 +1688,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1697,17 +1703,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1723,156 +1725,154 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
@@ -1880,7 +1880,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1889,6 +1889,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2237,11 +2238,18 @@
   <sheetPr/>
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="13.7890625" customWidth="1"/>
+    <col min="3" max="3" width="78.8984375" customWidth="1"/>
+    <col min="4" max="4" width="26.9453125" customWidth="1"/>
+    <col min="5" max="5" width="22.78125" customWidth="1"/>
+    <col min="6" max="6" width="64.9765625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
@@ -2539,7 +2547,7 @@
       <c r="E15" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2559,7 +2567,7 @@
       <c r="E16" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2639,7 +2647,7 @@
       <c r="E20" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2879,7 +2887,7 @@
       <c r="E32" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="4" t="s">
         <v>138</v>
       </c>
     </row>
@@ -3179,7 +3187,7 @@
       <c r="E47" t="s">
         <v>156</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="4" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3219,7 +3227,7 @@
       <c r="E49" t="s">
         <v>181</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="4" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3459,7 +3467,7 @@
       <c r="E61" t="s">
         <v>217</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F61" s="4" t="s">
         <v>218</v>
       </c>
     </row>
@@ -3619,7 +3627,7 @@
       <c r="E69" t="s">
         <v>249</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="F69" s="4" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4039,7 +4047,7 @@
       <c r="E90" t="s">
         <v>317</v>
       </c>
-      <c r="F90" s="3" t="s">
+      <c r="F90" s="4" t="s">
         <v>318</v>
       </c>
     </row>
@@ -4299,7 +4307,7 @@
       <c r="E103" t="s">
         <v>371</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F103" s="4" t="s">
         <v>372</v>
       </c>
     </row>
@@ -4419,7 +4427,7 @@
       <c r="E109" t="s">
         <v>392</v>
       </c>
-      <c r="F109" s="3" t="s">
+      <c r="F109" s="4" t="s">
         <v>393</v>
       </c>
     </row>

</xml_diff>